<commit_message>
Updated parts lists, updated folder names
Updated parts lists, updated folder names
</commit_message>
<xml_diff>
--- a/docs/build_instructions_deluxe.xlsx
+++ b/docs/build_instructions_deluxe.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="500" documentId="415E32CF7F9D79DA378485C62B6EEDB6DC1C7F04" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AA2D26A5-4C39-4C95-A5D8-E955380A2195}"/>
+  <xr:revisionPtr revIDLastSave="561" documentId="415E32CF7F9D79DA378485C62B6EEDB6DC1C7F04" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E2A71ED7-768F-4635-A928-C98523B83C87}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="case_1" sheetId="7" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="56">
   <si>
     <t>Amazon</t>
   </si>
@@ -91,9 +91,6 @@
     <t>M2.5 screws length=10mm ThreadPitch=0.45</t>
   </si>
   <si>
-    <t>Micro SD card</t>
-  </si>
-  <si>
     <t>Arvicka speakers</t>
   </si>
   <si>
@@ -112,9 +109,6 @@
     <t>Female-female jumper wires 30cm</t>
   </si>
   <si>
-    <t>Pi Shop</t>
-  </si>
-  <si>
     <t>Cost</t>
   </si>
   <si>
@@ -145,25 +139,13 @@
     <t xml:space="preserve">See instructions above. </t>
   </si>
   <si>
-    <t>Or Pi Shop SKU 1260</t>
-  </si>
-  <si>
     <t>Or search for "MakerSpot 4-Port Stackable USB Hub HAT"</t>
   </si>
   <si>
     <t>Or Amazon B00F7120TQ</t>
   </si>
   <si>
-    <t>If you have a crafting friend, they probably have some</t>
-  </si>
-  <si>
     <t>Prices will vary. Does not include tax, shipping.</t>
-  </si>
-  <si>
-    <t>Or upgrade to Amazon B06XWN9Q99 or any 16GB+ card</t>
-  </si>
-  <si>
-    <t>Or Amazon B077Y149DL or any physically small USB drive</t>
   </si>
   <si>
     <t>Other speakers no larger than 56W x 56D x 66H mm per speaker &amp; 
@@ -176,9 +158,6 @@
     <t>Or Amazon B06XQTHDRR</t>
   </si>
   <si>
-    <t>Or Amazon B07KJYR8K1 or search Amazon for KY-016</t>
-  </si>
-  <si>
     <t>Sticky back rubber feet (100 pieces)</t>
   </si>
   <si>
@@ -186,14 +165,48 @@
   </si>
   <si>
     <t>KY-040 rotary encoders (knobs)</t>
+  </si>
+  <si>
+    <t>Adafruit</t>
+  </si>
+  <si>
+    <t>16GB micro SD card</t>
+  </si>
+  <si>
+    <t>Or buy Amazon B06XWN9Q99 or other 16GB+ card</t>
+  </si>
+  <si>
+    <t>Or Amazon B07MDXBT87 or other physically small USB drive</t>
+  </si>
+  <si>
+    <t>Or buy at hobby store cheaper. If you have a crafting friend, they probably have some.</t>
+  </si>
+  <si>
+    <t>This is for a large kit of sensors, you only need KY-016. Or search KY-016, but note that almost all other sellers are in China.</t>
+  </si>
+  <si>
+    <t>AdaFruit</t>
+  </si>
+  <si>
+    <t>Premium Female/Female Jumper Wires - 40 x 6"</t>
+  </si>
+  <si>
+    <t>Or buy Amazon B07GCY6CH7</t>
+  </si>
+  <si>
+    <t>Or buy Amazon B00MARDJZ4</t>
+  </si>
+  <si>
+    <t>Or buy PiShop.us SKU 1052</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -277,7 +290,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -296,30 +309,6 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -373,17 +362,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -703,7 +690,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:D18"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -711,7 +698,7 @@
     <col min="1" max="1" width="37.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="47" style="1" customWidth="1"/>
+    <col min="4" max="4" width="61" style="1" customWidth="1"/>
     <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
@@ -723,10 +710,10 @@
         <v>5</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -740,7 +727,7 @@
         <v>69.28</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -748,13 +735,13 @@
         <v>14</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="C3" s="6">
-        <v>14.95</v>
+        <v>14</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -762,198 +749,202 @@
         <v>15</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="C4" s="6">
-        <v>6.2</v>
-      </c>
-      <c r="D4" s="10"/>
+        <v>7.5</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>0</v>
+      <c r="A5" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="C5" s="6">
-        <v>13.99</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>39</v>
+        <v>3.95</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="6">
-        <v>22.99</v>
+        <v>13.99</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="6">
-        <v>11.99</v>
-      </c>
-      <c r="D7" s="10"/>
+        <v>22.99</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="6">
-        <v>5.59</v>
+        <v>11.99</v>
       </c>
       <c r="D8" s="10"/>
     </row>
     <row r="9" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="6">
-        <v>4.75</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>43</v>
-      </c>
+        <v>6.72</v>
+      </c>
+      <c r="D9" s="10"/>
     </row>
     <row r="10" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="6">
+        <v>4.95</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="6">
-        <v>5.6</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
-        <v>21</v>
-      </c>
       <c r="B11" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C11" s="6">
+        <v>6.34</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="6">
         <v>19.989999999999998</v>
       </c>
-      <c r="D11" s="13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="6">
-        <v>9.99</v>
-      </c>
-      <c r="D12" s="10"/>
+      <c r="D12" s="13" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C13" s="6">
-        <v>5.99</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>46</v>
-      </c>
+        <v>9.99</v>
+      </c>
+      <c r="D13" s="10"/>
     </row>
     <row r="14" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C14" s="6">
-        <v>3.17</v>
+        <v>5.69</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C15" s="6">
-        <v>7.99</v>
+        <v>10.99</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C16" s="6">
-        <v>5.79</v>
-      </c>
-      <c r="D16" s="10"/>
-    </row>
-    <row r="17" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
+        <v>7.99</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="22" t="s">
         <v>0</v>
       </c>
       <c r="C17" s="6">
-        <v>6.99</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>48</v>
+        <v>17.989999999999998</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="16">
         <f>SUM(C2:C17)</f>
-        <v>215.25000000000003</v>
+        <v>234.35000000000005</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -962,21 +953,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" display="https://www.pishop.us/product/raspberry-pi-zero-wireless-wh-pre-soldered-header/" xr:uid="{021926D1-5A0F-423C-8CBF-D0BB6978B50E}"/>
-    <hyperlink ref="A4" r:id="rId2" display="https://www.pishop.us/product/microusb-power-adapter-international-plugs/" xr:uid="{5EF5033D-2001-4601-B1BD-5CDC177D730C}"/>
-    <hyperlink ref="A5" r:id="rId3" display="https://www.amazon.com/gp/product/B01IT1TLFQ/ref=oh_aui_detailpage_o01_s00?ie=UTF8&amp;psc=1" xr:uid="{413D6FAB-2DE2-40CF-91FE-4C22B722364B}"/>
-    <hyperlink ref="A6" r:id="rId4" display="https://www.amazon.com/gp/product/B00KGK5I38/ref=ox_sc_saved_title_3?smid=ATVPDKIKX0DER&amp;psc=1" xr:uid="{7CD94E18-5E56-4D94-A58E-DEF0573D5C9A}"/>
-    <hyperlink ref="A7" r:id="rId5" display="https://www.amazon.com/Sutemribor-Female-Spacer-Standoff-Assortment/dp/B075K3QBMX/ref=sr_1_4?ie=UTF8&amp;qid=1544322291&amp;sr=8-4&amp;keywords=M2.5+standoff" xr:uid="{EF899476-FE61-4947-82A1-01F6928A66A6}"/>
-    <hyperlink ref="A8" r:id="rId6" display="https://www.amazon.com/Machine-Finish-Phillips-M2-5-0-45-Threaded/dp/B00F33S93E/ref=sr_1_22?rps=1&amp;ie=UTF8&amp;qid=1544398707&amp;sr=8-22&amp;keywords=M2.5+screws+10mm&amp;refinements=p_85%3A2470955011" xr:uid="{029BC288-2440-4502-9532-12C8FDD4205A}"/>
-    <hyperlink ref="A9" r:id="rId7" xr:uid="{AE7EC994-D6BE-4623-9F6D-A4727D4345D2}"/>
-    <hyperlink ref="A10" r:id="rId8" display="https://www.amazon.com/SanDisk-16GB-Cruzer-Flash-Drive/dp/B07MDXBT87/ref=sr_1_10?keywords=Cruzer+8GB&amp;qid=1572121525&amp;s=electronics&amp;sr=1-10" xr:uid="{9A533D1E-D233-47BF-979E-16F459D06B87}"/>
-    <hyperlink ref="A11" r:id="rId9" display="https://www.amazon.com/gp/product/B01KC7WGQQ/ref=oh_aui_search_detailpage?ie=UTF8&amp;psc=1" xr:uid="{4C7D1439-1286-4238-8D81-286010A89FF3}"/>
-    <hyperlink ref="A12" r:id="rId10" display="https://www.amazon.com/gp/product/B01HMBKQNA/ref=oh_aui_search_detailpage?ie=UTF8&amp;psc=1" xr:uid="{3A39CDC9-6384-4F4B-859B-0F9B18770043}"/>
-    <hyperlink ref="A13" r:id="rId11" xr:uid="{E2EF51F2-2B6D-426C-B36E-4E42C09ECDC6}"/>
-    <hyperlink ref="A15" r:id="rId12" display="https://www.amazon.com/Tegg-KY-040-Encoder-clickable-Arduino/dp/B07QL6V4WP/ref=sr_1_11?keywords=KY-040&amp;qid=1572122001&amp;sr=8-11" xr:uid="{EA1A8E7F-41F7-406F-8645-EED638E412D8}"/>
-    <hyperlink ref="A16" r:id="rId13" xr:uid="{04D83557-E257-401E-B08D-315CEC806DC2}"/>
-    <hyperlink ref="A17" r:id="rId14" display="https://www.amazon.com/KY-016-Colors-Sensor-Arduino-Starter/dp/B0786CQD5P/ref=sr_1_1?keywords=KY-016&amp;qid=1572122200&amp;sr=8-1" xr:uid="{1B9A94FF-A19D-4B75-8874-3DC44290BA15}"/>
-    <hyperlink ref="A14" r:id="rId15" xr:uid="{55530A7A-F3D3-4EE2-BD90-428202C51155}"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{021926D1-5A0F-423C-8CBF-D0BB6978B50E}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{5EF5033D-2001-4601-B1BD-5CDC177D730C}"/>
+    <hyperlink ref="A6" r:id="rId3" display="https://www.amazon.com/gp/product/B01IT1TLFQ/ref=oh_aui_detailpage_o01_s00?ie=UTF8&amp;psc=1" xr:uid="{413D6FAB-2DE2-40CF-91FE-4C22B722364B}"/>
+    <hyperlink ref="A7" r:id="rId4" display="https://www.amazon.com/gp/product/B00KGK5I38/ref=ox_sc_saved_title_3?smid=ATVPDKIKX0DER&amp;psc=1" xr:uid="{7CD94E18-5E56-4D94-A58E-DEF0573D5C9A}"/>
+    <hyperlink ref="A8" r:id="rId5" display="https://www.amazon.com/Sutemribor-Female-Spacer-Standoff-Assortment/dp/B075K3QBMX/ref=sr_1_4?ie=UTF8&amp;qid=1544322291&amp;sr=8-4&amp;keywords=M2.5+standoff" xr:uid="{EF899476-FE61-4947-82A1-01F6928A66A6}"/>
+    <hyperlink ref="A9" r:id="rId6" display="https://www.amazon.com/Machine-Finish-Phillips-M2-5-0-45-Threaded/dp/B00F33S93E/ref=sr_1_22?rps=1&amp;ie=UTF8&amp;qid=1544398707&amp;sr=8-22&amp;keywords=M2.5+screws+10mm&amp;refinements=p_85%3A2470955011" xr:uid="{029BC288-2440-4502-9532-12C8FDD4205A}"/>
+    <hyperlink ref="A12" r:id="rId7" display="https://www.amazon.com/gp/product/B01KC7WGQQ/ref=oh_aui_search_detailpage?ie=UTF8&amp;psc=1" xr:uid="{4C7D1439-1286-4238-8D81-286010A89FF3}"/>
+    <hyperlink ref="A13" r:id="rId8" display="https://www.amazon.com/gp/product/B01HMBKQNA/ref=oh_aui_search_detailpage?ie=UTF8&amp;psc=1" xr:uid="{3A39CDC9-6384-4F4B-859B-0F9B18770043}"/>
+    <hyperlink ref="A14" r:id="rId9" xr:uid="{E2EF51F2-2B6D-426C-B36E-4E42C09ECDC6}"/>
+    <hyperlink ref="A16" r:id="rId10" display="https://www.amazon.com/Tegg-KY-040-Encoder-clickable-Arduino/dp/B07QL6V4WP/ref=sr_1_11?keywords=KY-040&amp;qid=1572122001&amp;sr=8-11" xr:uid="{EA1A8E7F-41F7-406F-8645-EED638E412D8}"/>
+    <hyperlink ref="A15" r:id="rId11" xr:uid="{55530A7A-F3D3-4EE2-BD90-428202C51155}"/>
+    <hyperlink ref="A10" r:id="rId12" xr:uid="{0206C24A-49D9-4B1F-88FC-D0BB515EBEF3}"/>
+    <hyperlink ref="A11" r:id="rId13" xr:uid="{51FA4659-6A94-494E-9F78-D7C18CB19413}"/>
+    <hyperlink ref="A17" r:id="rId14" xr:uid="{010DAD22-E559-4848-9F27-8B06AB015B93}"/>
+    <hyperlink ref="A5" r:id="rId15" xr:uid="{F638D896-B204-4959-9695-2F133FA9ECE8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId16"/>
@@ -988,7 +979,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1074,7 +1065,7 @@
         <v>25</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -1082,21 +1073,21 @@
         <v>14</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="C6" s="14">
         <v>10</v>
       </c>
       <c r="D6" s="6">
-        <v>14.95</v>
+        <v>14</v>
       </c>
       <c r="E6" s="6">
         <f t="shared" si="0"/>
-        <v>149.5</v>
+        <v>140</v>
       </c>
       <c r="F6" s="6">
         <f t="shared" si="1"/>
-        <v>14.95</v>
+        <v>14</v>
       </c>
       <c r="G6" s="10"/>
     </row>
@@ -1105,21 +1096,21 @@
         <v>15</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="C7" s="14">
         <v>10</v>
       </c>
       <c r="D7" s="6">
-        <v>6.2</v>
+        <v>7.5</v>
       </c>
       <c r="E7" s="6">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="F7" s="6">
         <f t="shared" si="1"/>
-        <v>6.2</v>
+        <v>7.5</v>
       </c>
       <c r="G7" s="10"/>
     </row>
@@ -1171,7 +1162,7 @@
     </row>
     <row r="10" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>10</v>
@@ -1194,7 +1185,7 @@
     </row>
     <row r="11" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>10</v>
@@ -1226,21 +1217,21 @@
         <v>1</v>
       </c>
       <c r="D12" s="6">
-        <v>5.59</v>
+        <v>6.72</v>
       </c>
       <c r="E12" s="6">
         <f t="shared" si="0"/>
-        <v>5.59</v>
+        <v>6.72</v>
       </c>
       <c r="F12" s="6">
         <f t="shared" si="1"/>
-        <v>0.55899999999999994</v>
+        <v>0.67199999999999993</v>
       </c>
       <c r="G12" s="10"/>
     </row>
     <row r="13" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>0</v>
@@ -1249,15 +1240,15 @@
         <v>10</v>
       </c>
       <c r="D13" s="6">
-        <v>4.75</v>
+        <v>4.95</v>
       </c>
       <c r="E13" s="6">
         <f t="shared" si="0"/>
-        <v>47.5</v>
+        <v>49.5</v>
       </c>
       <c r="F13" s="6">
         <f t="shared" si="1"/>
-        <v>4.75</v>
+        <v>4.95</v>
       </c>
       <c r="G13" s="10"/>
     </row>
@@ -1272,21 +1263,21 @@
         <v>10</v>
       </c>
       <c r="D14" s="6">
-        <v>5.6</v>
+        <v>6.34</v>
       </c>
       <c r="E14" s="6">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>63.4</v>
       </c>
       <c r="F14" s="6">
         <f t="shared" si="1"/>
-        <v>5.6</v>
+        <v>6.34</v>
       </c>
       <c r="G14" s="10"/>
     </row>
     <row r="15" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>0</v>
@@ -1309,7 +1300,7 @@
     </row>
     <row r="16" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>0</v>
@@ -1332,7 +1323,7 @@
     </row>
     <row r="17" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>0</v>
@@ -1341,21 +1332,21 @@
         <v>1</v>
       </c>
       <c r="D17" s="6">
-        <v>5.99</v>
+        <v>5.69</v>
       </c>
       <c r="E17" s="6">
         <f t="shared" si="0"/>
-        <v>5.99</v>
+        <v>5.69</v>
       </c>
       <c r="F17" s="6">
         <f t="shared" si="1"/>
-        <v>0.59899999999999998</v>
+        <v>0.56900000000000006</v>
       </c>
       <c r="G17" s="10"/>
     </row>
     <row r="18" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>0</v>
@@ -1364,42 +1355,42 @@
         <v>1</v>
       </c>
       <c r="D18" s="6">
-        <v>3.17</v>
+        <v>10.99</v>
       </c>
       <c r="E18" s="6">
         <f t="shared" si="0"/>
-        <v>3.17</v>
+        <v>10.99</v>
       </c>
       <c r="F18" s="6">
         <f t="shared" si="1"/>
-        <v>0.317</v>
+        <v>1.099</v>
       </c>
       <c r="G18" s="10"/>
     </row>
-    <row r="19" spans="1:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="23">
+        <v>44</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="24">
         <v>20</v>
       </c>
-      <c r="D19" s="24">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="E19" s="24">
+      <c r="D19" s="6">
+        <v>72</v>
+      </c>
+      <c r="E19" s="6">
         <v>11</v>
       </c>
-      <c r="F19" s="24">
+      <c r="F19" s="6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="G19" s="22"/>
+      <c r="G19" s="5"/>
     </row>
     <row r="20" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>10</v>
@@ -1422,7 +1413,7 @@
     </row>
     <row r="21" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>10</v>
@@ -1431,21 +1422,21 @@
         <v>1</v>
       </c>
       <c r="D21" s="6">
-        <v>1.86</v>
+        <v>1.92</v>
       </c>
       <c r="E21" s="6">
         <f t="shared" si="0"/>
-        <v>1.86</v>
+        <v>1.92</v>
       </c>
       <c r="F21" s="6">
         <f t="shared" si="1"/>
-        <v>0.186</v>
+        <v>0.192</v>
       </c>
       <c r="G21" s="10"/>
     </row>
     <row r="22" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="20" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>10</v>
@@ -1454,18 +1445,18 @@
         <v>1</v>
       </c>
       <c r="D22" s="6">
-        <v>1.0900000000000001</v>
+        <v>1.17</v>
       </c>
       <c r="E22" s="6">
         <f t="shared" si="0"/>
-        <v>1.0900000000000001</v>
+        <v>1.17</v>
       </c>
       <c r="F22" s="6">
         <f t="shared" si="1"/>
-        <v>0.10900000000000001</v>
+        <v>0.11699999999999999</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -1476,31 +1467,31 @@
       <c r="E23" s="17"/>
       <c r="F23" s="16">
         <f>SUM(F5:F22)</f>
-        <v>119.41399999999999</v>
+        <v>121.583</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1" display="https://www.pishop.us/product/raspberry-pi-zero-wireless-wh-pre-soldered-header/" xr:uid="{EBBDDE1D-AC2C-4209-B4A7-99DA11A03F82}"/>
-    <hyperlink ref="A7" r:id="rId2" display="https://www.pishop.us/product/microusb-power-adapter-international-plugs/" xr:uid="{62D64092-E9BE-44D3-BB7B-BAEDFC397478}"/>
-    <hyperlink ref="A8" r:id="rId3" display="https://www.amazon.com/gp/product/B01IT1TLFQ/ref=oh_aui_detailpage_o01_s00?ie=UTF8&amp;psc=1" xr:uid="{5A2F2652-302B-4AEA-B095-1658F3402F1E}"/>
-    <hyperlink ref="A9" r:id="rId4" display="https://www.amazon.com/gp/product/B00KGK5I38/ref=ox_sc_saved_title_3?smid=ATVPDKIKX0DER&amp;psc=1" xr:uid="{0EF4E5C1-2EBA-43A5-9B25-64D5E25E426C}"/>
-    <hyperlink ref="A11" r:id="rId5" xr:uid="{8FED7CA6-75E9-41D1-86E1-F4724E7A6F90}"/>
-    <hyperlink ref="A12" r:id="rId6" display="https://www.amazon.com/Machine-Finish-Phillips-M2-5-0-45-Threaded/dp/B00F33S93E/ref=sr_1_22?rps=1&amp;ie=UTF8&amp;qid=1544398707&amp;sr=8-22&amp;keywords=M2.5+screws+10mm&amp;refinements=p_85%3A2470955011" xr:uid="{13A44263-8D55-4F4F-BE4B-FE6B8E6578BF}"/>
-    <hyperlink ref="A13" r:id="rId7" xr:uid="{DA08ECA4-980D-4ADA-9524-6AAFBF559DD4}"/>
-    <hyperlink ref="A14" r:id="rId8" display="https://www.amazon.com/SanDisk-16GB-Cruzer-Flash-Drive/dp/B07MDXBT87/ref=sr_1_10?keywords=Cruzer+8GB&amp;qid=1572121525&amp;s=electronics&amp;sr=1-10" xr:uid="{9BBEC281-ED69-4FB8-898D-71E81CB1A53B}"/>
-    <hyperlink ref="A15" r:id="rId9" display="https://www.amazon.com/gp/product/B01KC7WGQQ/ref=oh_aui_search_detailpage?ie=UTF8&amp;psc=1" xr:uid="{A535EA10-1ECA-42F8-8BCF-1CE2BACF23E4}"/>
-    <hyperlink ref="A16" r:id="rId10" display="https://www.amazon.com/gp/product/B01HMBKQNA/ref=oh_aui_search_detailpage?ie=UTF8&amp;psc=1" xr:uid="{7253BB0C-B5CC-49FC-8373-607CA592AC27}"/>
-    <hyperlink ref="A17" r:id="rId11" xr:uid="{5BE6FC4E-DB94-48B0-85C7-7D18DD77B2E3}"/>
-    <hyperlink ref="A20" r:id="rId12" xr:uid="{54B370DD-34BC-41EF-8506-D508D936AC55}"/>
-    <hyperlink ref="A18" r:id="rId13" xr:uid="{2EB770D9-DE3A-4650-85D5-08B4ECBD8850}"/>
-    <hyperlink ref="A10" r:id="rId14" xr:uid="{A30D3F27-789F-47E8-BF73-085292AEA9C8}"/>
-    <hyperlink ref="A21" r:id="rId15" display="KY-016 indicator LED" xr:uid="{DEFC484D-5D94-4037-8035-4C92DA564D88}"/>
-    <hyperlink ref="A22" r:id="rId16" display="Sticky back rubber feet" xr:uid="{A6E2A975-8CB6-4A23-973C-5F2B4C8EC89A}"/>
-    <hyperlink ref="A19" r:id="rId17" display="https://www.aliexpress.com/item/599712551.html?spm=a2g0o.productlist.0.0.e62e585aMTYzjg&amp;algo_pvid=f1759f37-1668-4260-a1ec-19fa8f3121f1&amp;algo_expid=f1759f37-1668-4260-a1ec-19fa8f3121f1-3&amp;btsid=0ab6f82215868356579722627e4fa1&amp;ws_ab_test=searchweb0_0,searchweb201602_,searchweb201603_" xr:uid="{E2A763BB-4D86-4B19-8749-7360249C4777}"/>
+    <hyperlink ref="A8" r:id="rId1" display="https://www.amazon.com/gp/product/B01IT1TLFQ/ref=oh_aui_detailpage_o01_s00?ie=UTF8&amp;psc=1" xr:uid="{5A2F2652-302B-4AEA-B095-1658F3402F1E}"/>
+    <hyperlink ref="A9" r:id="rId2" display="https://www.amazon.com/gp/product/B00KGK5I38/ref=ox_sc_saved_title_3?smid=ATVPDKIKX0DER&amp;psc=1" xr:uid="{0EF4E5C1-2EBA-43A5-9B25-64D5E25E426C}"/>
+    <hyperlink ref="A11" r:id="rId3" xr:uid="{8FED7CA6-75E9-41D1-86E1-F4724E7A6F90}"/>
+    <hyperlink ref="A12" r:id="rId4" display="https://www.amazon.com/Machine-Finish-Phillips-M2-5-0-45-Threaded/dp/B00F33S93E/ref=sr_1_22?rps=1&amp;ie=UTF8&amp;qid=1544398707&amp;sr=8-22&amp;keywords=M2.5+screws+10mm&amp;refinements=p_85%3A2470955011" xr:uid="{13A44263-8D55-4F4F-BE4B-FE6B8E6578BF}"/>
+    <hyperlink ref="A15" r:id="rId5" display="https://www.amazon.com/gp/product/B01KC7WGQQ/ref=oh_aui_search_detailpage?ie=UTF8&amp;psc=1" xr:uid="{A535EA10-1ECA-42F8-8BCF-1CE2BACF23E4}"/>
+    <hyperlink ref="A16" r:id="rId6" display="https://www.amazon.com/gp/product/B01HMBKQNA/ref=oh_aui_search_detailpage?ie=UTF8&amp;psc=1" xr:uid="{7253BB0C-B5CC-49FC-8373-607CA592AC27}"/>
+    <hyperlink ref="A20" r:id="rId7" xr:uid="{54B370DD-34BC-41EF-8506-D508D936AC55}"/>
+    <hyperlink ref="A18" r:id="rId8" xr:uid="{2EB770D9-DE3A-4650-85D5-08B4ECBD8850}"/>
+    <hyperlink ref="A10" r:id="rId9" xr:uid="{A30D3F27-789F-47E8-BF73-085292AEA9C8}"/>
+    <hyperlink ref="A21" r:id="rId10" display="KY-016 indicator LED" xr:uid="{DEFC484D-5D94-4037-8035-4C92DA564D88}"/>
+    <hyperlink ref="A22" r:id="rId11" display="Sticky back rubber feet" xr:uid="{A6E2A975-8CB6-4A23-973C-5F2B4C8EC89A}"/>
+    <hyperlink ref="A19" r:id="rId12" display="https://www.aliexpress.com/item/599712551.html?spm=a2g0o.productlist.0.0.e62e585aMTYzjg&amp;algo_pvid=f1759f37-1668-4260-a1ec-19fa8f3121f1&amp;algo_expid=f1759f37-1668-4260-a1ec-19fa8f3121f1-3&amp;btsid=0ab6f82215868356579722627e4fa1&amp;ws_ab_test=searchweb0_0,searchweb201602_,searchweb201603_" xr:uid="{E2A763BB-4D86-4B19-8749-7360249C4777}"/>
+    <hyperlink ref="A13" r:id="rId13" xr:uid="{6B09B683-8BC8-4F08-AC88-0ABAE3672F98}"/>
+    <hyperlink ref="A14" r:id="rId14" xr:uid="{FD5E15DD-8CA5-418A-8152-C5896D463D17}"/>
+    <hyperlink ref="A17" r:id="rId15" xr:uid="{DCBC963C-C235-4848-B6D3-418F17DCDD1E}"/>
+    <hyperlink ref="A6" r:id="rId16" xr:uid="{70EFE953-062F-4127-8206-67FA84B92838}"/>
+    <hyperlink ref="A7" r:id="rId17" xr:uid="{1BC8ABF0-4431-41A3-BB3C-2F914BCF5092}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId18"/>

</xml_diff>

<commit_message>
updated folder names and file names to better match product names
updated folder names and file names to better match product names
</commit_message>
<xml_diff>
--- a/docs/build_instructions_deluxe.xlsx
+++ b/docs/build_instructions_deluxe.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="561" documentId="415E32CF7F9D79DA378485C62B6EEDB6DC1C7F04" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E2A71ED7-768F-4635-A928-C98523B83C87}"/>
+  <xr:revisionPtr revIDLastSave="565" documentId="415E32CF7F9D79DA378485C62B6EEDB6DC1C7F04" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8143DEB4-99DD-4906-916E-D67C1070B301}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -115,9 +115,6 @@
     <t>TOTAL</t>
   </si>
   <si>
-    <t>Or order 10+ from Ponoko for @$43.71</t>
-  </si>
-  <si>
     <t>M2.5x15mm + 6mm standoffs (50 pieces)</t>
   </si>
   <si>
@@ -198,6 +195,9 @@
   </si>
   <si>
     <t>Or buy PiShop.us SKU 1052</t>
+  </si>
+  <si>
+    <t>Or order 10+ from Ponoko for @$51.21</t>
   </si>
 </sst>
 </file>
@@ -690,7 +690,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -713,7 +713,7 @@
         <v>26</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -724,10 +724,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="6">
-        <v>69.28</v>
+        <v>84.77</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -735,13 +735,13 @@
         <v>14</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="6">
         <v>14</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -749,27 +749,27 @@
         <v>15</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="6">
         <v>7.5</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="6">
         <v>3.95</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -783,7 +783,7 @@
         <v>13.99</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -797,7 +797,7 @@
         <v>22.99</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -826,7 +826,7 @@
     </row>
     <row r="10" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>0</v>
@@ -835,7 +835,7 @@
         <v>4.95</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -849,7 +849,7 @@
         <v>6.34</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -863,7 +863,7 @@
         <v>19.989999999999998</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -889,7 +889,7 @@
         <v>5.69</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -903,7 +903,7 @@
         <v>10.99</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -917,7 +917,7 @@
         <v>7.99</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -931,7 +931,7 @@
         <v>17.989999999999998</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -941,10 +941,10 @@
       <c r="B18" s="5"/>
       <c r="C18" s="16">
         <f>SUM(C2:C17)</f>
-        <v>234.35000000000005</v>
+        <v>249.84000000000003</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -979,7 +979,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1065,7 +1065,7 @@
         <v>25</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -1073,7 +1073,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" s="14">
         <v>10</v>
@@ -1096,7 +1096,7 @@
         <v>15</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" s="14">
         <v>10</v>
@@ -1162,7 +1162,7 @@
     </row>
     <row r="10" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>10</v>
@@ -1185,7 +1185,7 @@
     </row>
     <row r="11" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>10</v>
@@ -1231,7 +1231,7 @@
     </row>
     <row r="13" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>0</v>
@@ -1300,7 +1300,7 @@
     </row>
     <row r="16" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>0</v>
@@ -1369,7 +1369,7 @@
     </row>
     <row r="19" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>10</v>
@@ -1413,7 +1413,7 @@
     </row>
     <row r="21" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>10</v>
@@ -1436,7 +1436,7 @@
     </row>
     <row r="22" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>10</v>
@@ -1456,7 +1456,7 @@
         <v>0.11699999999999999</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -1470,7 +1470,7 @@
         <v>121.583</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated parts list, including pricing
updated parts list, including pricing
</commit_message>
<xml_diff>
--- a/docs/build_instructions_deluxe.xlsx
+++ b/docs/build_instructions_deluxe.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="565" documentId="415E32CF7F9D79DA378485C62B6EEDB6DC1C7F04" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8143DEB4-99DD-4906-916E-D67C1070B301}"/>
+  <xr:revisionPtr revIDLastSave="566" documentId="415E32CF7F9D79DA378485C62B6EEDB6DC1C7F04" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{17EED721-A066-4AA4-99B1-5C60516694A0}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="case_1" sheetId="7" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="57">
   <si>
     <t>Amazon</t>
   </si>
@@ -179,9 +179,6 @@
     <t>Or buy at hobby store cheaper. If you have a crafting friend, they probably have some.</t>
   </si>
   <si>
-    <t>This is for a large kit of sensors, you only need KY-016. Or search KY-016, but note that almost all other sellers are in China.</t>
-  </si>
-  <si>
     <t>AdaFruit</t>
   </si>
   <si>
@@ -198,6 +195,12 @@
   </si>
   <si>
     <t>Or order 10+ from Ponoko for @$51.21</t>
+  </si>
+  <si>
+    <t>Banggood</t>
+  </si>
+  <si>
+    <t>ALLOW 3+ WEEKS TO ARRIVE FROM CHINA. Due to COVID, it's hard to find these in the US. You can get it quickly from Amazon B07KJYR8K1, but costs $18.</t>
   </si>
 </sst>
 </file>
@@ -689,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0E12D50-D309-4C94-883F-34F0FBB95462}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -741,7 +744,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -755,21 +758,21 @@
         <v>7.5</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" s="6">
         <v>3.95</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -925,13 +928,13 @@
         <v>2</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="C17" s="6">
-        <v>17.989999999999998</v>
+        <v>4.2699999999999996</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -941,7 +944,7 @@
       <c r="B18" s="5"/>
       <c r="C18" s="16">
         <f>SUM(C2:C17)</f>
-        <v>249.84000000000003</v>
+        <v>236.12000000000003</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>37</v>
@@ -966,8 +969,8 @@
     <hyperlink ref="A15" r:id="rId11" xr:uid="{55530A7A-F3D3-4EE2-BD90-428202C51155}"/>
     <hyperlink ref="A10" r:id="rId12" xr:uid="{0206C24A-49D9-4B1F-88FC-D0BB515EBEF3}"/>
     <hyperlink ref="A11" r:id="rId13" xr:uid="{51FA4659-6A94-494E-9F78-D7C18CB19413}"/>
-    <hyperlink ref="A17" r:id="rId14" xr:uid="{010DAD22-E559-4848-9F27-8B06AB015B93}"/>
-    <hyperlink ref="A5" r:id="rId15" xr:uid="{F638D896-B204-4959-9695-2F133FA9ECE8}"/>
+    <hyperlink ref="A5" r:id="rId14" xr:uid="{F638D896-B204-4959-9695-2F133FA9ECE8}"/>
+    <hyperlink ref="A17" r:id="rId15" xr:uid="{A142151C-D640-4EBA-8646-1657A12EAEF0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId16"/>
@@ -978,8 +981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD35BB53-6D32-4D96-AF53-91579E0632D6}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1065,7 +1068,7 @@
         <v>25</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>